<commit_message>
version v3 funcionando horarios correctamente
</commit_message>
<xml_diff>
--- a/sistema de registro de docentes/Resources/sportsc.xlsx
+++ b/sistema de registro de docentes/Resources/sportsc.xlsx
@@ -689,7 +689,7 @@
       <x:selection activeCell="B10" sqref="B10"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="14.085625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="14.210625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
     <x:col min="1" max="1" width="11.109375" style="0" customWidth="1"/>
     <x:col min="2" max="4" width="22" style="0" customWidth="1"/>
@@ -956,7 +956,7 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="Q5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1023,12 +1023,12 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="M2" r:id="rId14"/>
-    <x:hyperlink ref="M3" r:id="rId15"/>
-    <x:hyperlink ref="M4" r:id="rId16"/>
-    <x:hyperlink ref="P4" r:id="rId17"/>
-    <x:hyperlink ref="P3" r:id="rId18"/>
-    <x:hyperlink ref="P2" r:id="rId19"/>
+    <x:hyperlink ref="M2" r:id="rId12"/>
+    <x:hyperlink ref="M3" r:id="rId13"/>
+    <x:hyperlink ref="M4" r:id="rId20"/>
+    <x:hyperlink ref="P4" r:id="rId21"/>
+    <x:hyperlink ref="P3" r:id="rId22"/>
+    <x:hyperlink ref="P2" r:id="rId23"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>